<commit_message>
basic stt* upload added
</commit_message>
<xml_diff>
--- a/src/main/resources/Batch.xlsx
+++ b/src/main/resources/Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="6950"/>
+    <workbookView windowWidth="18530" windowHeight="6950" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LookupTemplate" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>Filed Type</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Please fill the valid detail for fast upload</t>
+  </si>
+  <si>
+    <t>Please enter the same drop down value which showing on web screen</t>
   </si>
 </sst>
 </file>
@@ -155,8 +158,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -183,15 +186,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,19 +211,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,32 +224,16 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,6 +253,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -298,15 +294,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,21 +332,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,67 +346,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,114 +527,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,30 +551,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,6 +595,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -632,17 +646,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -652,148 +655,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1074,7 +1077,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1168,10 +1171,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1500,9 +1503,17 @@
       </c>
       <c r="C35" s="4"/>
     </row>
+    <row r="36" ht="13" customHeight="1" spans="2:4">
+      <c r="B36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>